<commit_message>
added first row to db schedule excel file
</commit_message>
<xml_diff>
--- a/enigma.xlsx
+++ b/enigma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\gitrepos\Enigma-Bombe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2214D3EC-34CA-41E8-B7E4-7ED81AECF7B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDE8A2A-DDA6-4C92-86C4-62E635480AA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44440" yWindow="260" windowWidth="28800" windowHeight="15440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8295" yWindow="3840" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -354,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -365,7 +365,7 @@
     <col min="1" max="16384" width="18.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -379,12 +379,21 @@
         <v>1</v>
       </c>
       <c r="E1" s="1">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1">
         <v>2</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="1">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed what bombe function return statements
</commit_message>
<xml_diff>
--- a/enigma.xlsx
+++ b/enigma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\gitrepos\Enigma-Bombe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDE8A2A-DDA6-4C92-86C4-62E635480AA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FCDA73-7AF7-4695-9145-6E7E0A224B5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8295" yWindow="3840" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1275" yWindow="2895" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>ABCDEHIJKL</t>
   </si>
@@ -34,16 +34,52 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,9 +105,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -354,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -366,8 +405,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
-        <v>1</v>
+      <c r="A1" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -397,7 +436,53 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made fixes to createEnigmaSchedule, and added option to fill the Enigma database in CreateDB
</commit_message>
<xml_diff>
--- a/enigma.xlsx
+++ b/enigma.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\gitrepos\Enigma-Bombe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FCDA73-7AF7-4695-9145-6E7E0A224B5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B01615-E9A5-416C-B1A8-61FAB8748F86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="2895" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,45 +25,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>ABCDEHIJKL</t>
-  </si>
-  <si>
-    <t>MNOPQRSTUV</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
   <si>
     <t>B</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>ABCDEFGHJK</t>
+  </si>
+  <si>
+    <t>LMNOPQRSTU</t>
+  </si>
+  <si>
+    <t>LSFKOWERFQ</t>
+  </si>
+  <si>
+    <t>RTIKHJSDFX</t>
+  </si>
+  <si>
+    <t>CRDGNYWAXU</t>
+  </si>
+  <si>
+    <t>QLSOFIAPXV</t>
+  </si>
+  <si>
+    <t>AOPSDVXCZW</t>
+  </si>
+  <si>
+    <t>SFLZKYEBEH</t>
+  </si>
+  <si>
+    <t>EIROFDSAGC</t>
+  </si>
+  <si>
+    <t>LCKSPDOAEV</t>
+  </si>
+  <si>
+    <t>WOSPDFCLGZ</t>
+  </si>
+  <si>
+    <t>QRXAFGHLEV</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,84 +405,328 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
+      <c r="A1" s="2">
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1">
         <v>1</v>
       </c>
       <c r="E1" s="1">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1">
         <v>2</v>
       </c>
       <c r="G1" s="1">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1">
+        <v>4</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>11</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>5</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1">
+        <v>18</v>
+      </c>
+      <c r="F5" s="1">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>14</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>8</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1">
-        <v>2</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1">
+        <v>22</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>15</v>
+      </c>
+      <c r="H7" s="1">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1">
+        <v>5</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="E8" s="1">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1">
+        <v>11</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+      <c r="E10" s="1">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2</v>
+      </c>
+      <c r="G10" s="1">
+        <v>24</v>
+      </c>
+      <c r="H10" s="1">
+        <v>5</v>
+      </c>
+      <c r="I10" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made changes to plugboard values in excel file to fix errors
</commit_message>
<xml_diff>
--- a/enigma.xlsx
+++ b/enigma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\gitrepos\Enigma-Bombe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B01615-E9A5-416C-B1A8-61FAB8748F86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47AC31A-82CE-462B-B246-8167407E396C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="2895" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3675" yWindow="2355" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>B</t>
   </si>
@@ -36,34 +36,52 @@
     <t>LMNOPQRSTU</t>
   </si>
   <si>
-    <t>LSFKOWERFQ</t>
-  </si>
-  <si>
-    <t>RTIKHJSDFX</t>
-  </si>
-  <si>
-    <t>CRDGNYWAXU</t>
-  </si>
-  <si>
-    <t>QLSOFIAPXV</t>
-  </si>
-  <si>
-    <t>AOPSDVXCZW</t>
-  </si>
-  <si>
-    <t>SFLZKYEBEH</t>
-  </si>
-  <si>
-    <t>EIROFDSAGC</t>
-  </si>
-  <si>
-    <t>LCKSPDOAEV</t>
-  </si>
-  <si>
-    <t>WOSPDFCLGZ</t>
-  </si>
-  <si>
-    <t>QRXAFGHLEV</t>
+    <t>QWERTYUIOP</t>
+  </si>
+  <si>
+    <t>LKJHGFDSAZ</t>
+  </si>
+  <si>
+    <t>ZXCVBNMLKJ</t>
+  </si>
+  <si>
+    <t>HGFDSAPOIU</t>
+  </si>
+  <si>
+    <t>QAZWSXEDCR</t>
+  </si>
+  <si>
+    <t>FVTGBYHNUJ</t>
+  </si>
+  <si>
+    <t>QZECTBUMIL</t>
+  </si>
+  <si>
+    <t>PLOKIJUHYG</t>
+  </si>
+  <si>
+    <t>ALQPWODJUR</t>
+  </si>
+  <si>
+    <t>NTIGFUDOWQ</t>
+  </si>
+  <si>
+    <t>LSIDUCBKEQ</t>
+  </si>
+  <si>
+    <t>UBHVGYCXTA</t>
+  </si>
+  <si>
+    <t>PQLAMZSUDI</t>
+  </si>
+  <si>
+    <t>YUIKJHBNML</t>
+  </si>
+  <si>
+    <t>EORPFLSABN</t>
+  </si>
+  <si>
+    <t>DOFVKCLXQM</t>
   </si>
 </sst>
 </file>
@@ -396,7 +414,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,10 +555,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -569,10 +587,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -601,10 +619,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D7" s="1">
         <v>4</v>
@@ -633,10 +651,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1">
         <v>5</v>
@@ -665,10 +683,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1">
         <v>2</v>
@@ -697,10 +715,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1">
         <v>4</v>

</xml_diff>